<commit_message>
added the weekly forma and the biweekly forms
</commit_message>
<xml_diff>
--- a/config-nssd-migration-perinatal_workflow/forms/app/psupp_biweekly_visit.xlsx
+++ b/config-nssd-migration-perinatal_workflow/forms/app/psupp_biweekly_visit.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="123">
   <si>
     <t>type</t>
   </si>
@@ -451,10 +451,10 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>PSuPP Home visit</t>
-  </si>
-  <si>
-    <t>psupp_home_visit</t>
+    <t>PSuPP Biweekly visit</t>
+  </si>
+  <si>
+    <t>psupp_biweekly_visit</t>
   </si>
   <si>
     <t>pages</t>
@@ -464,24 +464,6 @@
   </si>
   <si>
     <t>en</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Cambria"/>
-        <color theme="1"/>
-        <sz val="8.0"/>
-      </rPr>
-      <t xml:space="preserve">PSuPP Home </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="8.0"/>
-      </rPr>
-      <t>फारम</t>
-    </r>
   </si>
   <si>
     <t>ne</t>
@@ -2303,7 +2285,7 @@
     </row>
     <row r="3">
       <c r="A3" s="23" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>118</v>
@@ -2319,7 +2301,7 @@
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4">

</xml_diff>